<commit_message>
Added POM structure of ROBOT
</commit_message>
<xml_diff>
--- a/SauceDemo_Practice/Resources/SauceDemoDatas.xlsx
+++ b/SauceDemo_Practice/Resources/SauceDemoDatas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RobotFramework-2\SauceDemo_Practice\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDFD7E5-4CA7-44FE-B1EF-9B5CDF740308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCC4114-1768-4037-8C8B-75B1C1CCA14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>${Username}</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -90,10 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,11 +429,29 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>